<commit_message>
Updated Week numbers on time sheets
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week4.xlsx
+++ b/Admin/Gaby/TimeSheet_Week4.xlsx
@@ -86,10 +86,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-mmm"/>
-    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -267,7 +266,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,10 +355,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -426,25 +425,25 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>44459</v>
+        <v>44452</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>44460</v>
+        <v>44453</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>44461</v>
+        <v>44454</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>44462</v>
+        <v>44455</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>44463</v>
+        <v>44456</v>
       </c>
       <c r="G5" s="7" t="n">
-        <v>44464</v>
+        <v>44457</v>
       </c>
       <c r="H5" s="6" t="n">
-        <v>44465</v>
+        <v>44458</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>6</v>
@@ -465,7 +464,6 @@
       <c r="G6" s="12"/>
       <c r="H6" s="11"/>
       <c r="I6" s="13" t="n">
-        <f aca="false">SUM(B6:H6)</f>
         <v>1</v>
       </c>
       <c r="J6" s="9"/>
@@ -493,14 +491,15 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
       <c r="H8" s="11"/>
       <c r="I8" s="13" t="n">
-        <f aca="false">SUM(B8:H8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="9"/>
     </row>
@@ -518,7 +517,6 @@
       <c r="G9" s="12"/>
       <c r="H9" s="11"/>
       <c r="I9" s="13" t="n">
-        <f aca="false">SUM(B9:H9)</f>
         <v>1</v>
       </c>
       <c r="J9" s="9"/>
@@ -527,17 +525,16 @@
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="11"/>
+      <c r="H10" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="I10" s="13" t="n">
-        <f aca="false">SUM(B10:H10)</f>
         <v>1</v>
       </c>
       <c r="J10" s="9"/>
@@ -556,7 +553,7 @@
       </c>
       <c r="D11" s="13" t="n">
         <f aca="false">SUM(D6:D9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="13" t="n">
         <f aca="false">SUM(E6:E9)</f>
@@ -572,11 +569,11 @@
       </c>
       <c r="H11" s="13" t="n">
         <f aca="false">SUM(H6:H10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="13" t="n">
         <f aca="false">SUM(I6:I10)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>